<commit_message>
Refactorizacion de estructura de scrapping
</commit_message>
<xml_diff>
--- a/clima.xlsx
+++ b/clima.xlsx
@@ -458,12 +458,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2 Ago</t>
+          <t>8 Ago</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>36° / 23°</t>
+          <t>38° / 23°</t>
         </is>
       </c>
     </row>
@@ -475,97 +475,97 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3 Ago</t>
+          <t>9 Ago</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>36° / 22°</t>
+          <t>36° / 23°</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Domingo</t>
+          <t>Sábado</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4 Ago</t>
+          <t>10 Ago</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>37° / 22°</t>
+          <t>36° / 23°</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Lunes</t>
+          <t>Domingo</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5 Ago</t>
+          <t>11 Ago</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>37° / 23°</t>
+          <t>37° / 22°</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Martes</t>
+          <t>Lunes</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6 Ago</t>
+          <t>12 Ago</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>38° / 23°</t>
+          <t>37° / 21°</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Miércoles</t>
+          <t>Martes</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7 Ago</t>
+          <t>13 Ago</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>38° / 23°</t>
+          <t>37° / 22°</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Jueves</t>
+          <t>Miércoles</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>8 Ago</t>
+          <t>14 Ago</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>37° / 24°</t>
+          <t>37° / 23°</t>
         </is>
       </c>
     </row>

</xml_diff>